<commit_message>
pushing files for the project management
</commit_message>
<xml_diff>
--- a/CMS/Build-Strategy-and-Estimates/ASQ Build Plan.xlsx
+++ b/CMS/Build-Strategy-and-Estimates/ASQ Build Plan.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
     <sheet name="WBS (Inherited&amp;Updated)" sheetId="4" r:id="rId2"/>
-    <sheet name="Estimation" sheetId="2" r:id="rId3"/>
+    <sheet name="Work Estimation" sheetId="2" r:id="rId3"/>
+    <sheet name="Budget" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
   <si>
     <t>Initial Work</t>
   </si>
@@ -640,12 +641,66 @@
   <si>
     <t>3.2.2 Bulk Import Questions</t>
   </si>
+  <si>
+    <t>Development Cost</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>System Architect</t>
+  </si>
+  <si>
+    <t>Developers</t>
+  </si>
+  <si>
+    <t>QA Team</t>
+  </si>
+  <si>
+    <t>Weekly Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Team Member</t>
+  </si>
+  <si>
+    <t>No.s</t>
+  </si>
+  <si>
+    <t>Project Budget</t>
+  </si>
+  <si>
+    <t>Item Description</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Buffer &amp; Overhead</t>
+  </si>
+  <si>
+    <t>Startup Discount</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Project is expect to be delivered in 12 weeks time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,6 +768,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -764,7 +835,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -884,11 +955,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -905,9 +1024,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1038,6 +1154,67 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1439,725 +1616,725 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="50" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="2.28515625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" style="51" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="51" customWidth="1"/>
-    <col min="8" max="8" width="2.140625" style="51" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="51" customWidth="1"/>
-    <col min="10" max="10" width="2.140625" style="51" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="51" customWidth="1"/>
-    <col min="12" max="12" width="2.140625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="12" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" style="51" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="12" customWidth="1"/>
-    <col min="16" max="16" width="2.7109375" style="51" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="51" customWidth="1"/>
-    <col min="18" max="18" width="2.7109375" style="51" customWidth="1"/>
-    <col min="19" max="19" width="2.7109375" style="12" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" style="52" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="15.7109375" style="49" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="2.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="50" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="50" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" style="50" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="50" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" style="50" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="50" customWidth="1"/>
+    <col min="12" max="12" width="2.140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="11" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="50" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="11" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="50" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="50" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="50" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" style="11" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="51" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="11"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="10"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="13"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" spans="1:20" ht="34.5" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="15" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="9" customHeight="1" thickBot="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="19"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="18"/>
     </row>
     <row r="5" spans="1:20" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="22" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="24" t="s">
+      <c r="N5" s="8"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="9" customHeight="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="28"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="27"/>
     </row>
     <row r="7" spans="1:20" ht="9" customHeight="1" thickBot="1">
-      <c r="A7" s="29"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="15"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="14"/>
     </row>
     <row r="8" spans="1:20" ht="30" customHeight="1" thickBot="1">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="30" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="32"/>
-      <c r="O8" s="30" t="s">
+      <c r="N8" s="31"/>
+      <c r="O8" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="24" t="s">
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="23" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="9" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="28"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="27"/>
     </row>
     <row r="10" spans="1:20" ht="9" customHeight="1" thickBot="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="15"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="14"/>
     </row>
     <row r="11" spans="1:20" ht="36" customHeight="1" thickBot="1">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="33" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33" t="s">
+      <c r="D11" s="33"/>
+      <c r="E11" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="36" t="s">
+      <c r="H11" s="36"/>
+      <c r="I11" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="36" t="s">
+      <c r="J11" s="36"/>
+      <c r="K11" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="37"/>
-      <c r="M11" s="33" t="s">
+      <c r="L11" s="36"/>
+      <c r="M11" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="N11" s="35"/>
-      <c r="O11" s="33" t="s">
+      <c r="N11" s="34"/>
+      <c r="O11" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="33" t="s">
+      <c r="P11" s="34"/>
+      <c r="Q11" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="R11" s="35"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="24" t="s">
+      <c r="R11" s="34"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="9" customHeight="1" thickBot="1">
-      <c r="A12" s="39"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="40"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="39"/>
     </row>
     <row r="13" spans="1:20" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A13" s="41"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="42" t="s">
+      <c r="A13" s="40"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="42" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44" t="s">
+      <c r="F13" s="42"/>
+      <c r="G13" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="44" t="s">
+      <c r="H13" s="34"/>
+      <c r="I13" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="55" t="s">
+      <c r="J13" s="34"/>
+      <c r="K13" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="33" t="s">
+      <c r="L13" s="34"/>
+      <c r="M13" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="35"/>
-      <c r="O13" s="45" t="s">
+      <c r="N13" s="34"/>
+      <c r="O13" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="44" t="s">
+      <c r="P13" s="34"/>
+      <c r="Q13" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="R13" s="35"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="46"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="1:20" ht="9" customHeight="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="40"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="39"/>
     </row>
     <row r="15" spans="1:20" ht="39.75" customHeight="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="42" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="44" t="s">
+      <c r="F15" s="34"/>
+      <c r="G15" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="44" t="s">
+      <c r="H15" s="34"/>
+      <c r="I15" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="42" t="s">
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N15" s="35"/>
-      <c r="O15" s="55" t="s">
+      <c r="N15" s="34"/>
+      <c r="O15" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="55" t="s">
+      <c r="P15" s="34"/>
+      <c r="Q15" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="R15" s="35"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="46"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="45"/>
     </row>
     <row r="16" spans="1:20" ht="9" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="40"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="39"/>
     </row>
     <row r="17" spans="1:20" ht="38.25" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="47"/>
-      <c r="E17" s="54" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="46"/>
+      <c r="E17" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="44" t="s">
+      <c r="F17" s="34"/>
+      <c r="G17" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="35"/>
-      <c r="I17" s="44" t="s">
+      <c r="H17" s="34"/>
+      <c r="I17" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="55" t="s">
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="46"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="45"/>
     </row>
     <row r="18" spans="1:20" ht="9" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="40"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="39"/>
     </row>
     <row r="19" spans="1:20" ht="28.5" customHeight="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="47"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="44" t="s">
+      <c r="A19" s="40"/>
+      <c r="B19" s="46"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="46"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="45"/>
     </row>
     <row r="20" spans="1:20" ht="9" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="40"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="39"/>
     </row>
     <row r="21" spans="1:20" ht="28.5" customHeight="1">
-      <c r="A21" s="41"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="46"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="45"/>
     </row>
     <row r="22" spans="1:20" ht="9" customHeight="1">
-      <c r="A22" s="39"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="40"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="39"/>
     </row>
     <row r="23" spans="1:20" ht="28.5" customHeight="1">
-      <c r="A23" s="41"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="46"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="45"/>
     </row>
     <row r="24" spans="1:20" ht="9" customHeight="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="40"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="39"/>
     </row>
     <row r="25" spans="1:20" ht="28.5" customHeight="1">
-      <c r="A25" s="41"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="46"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="45"/>
     </row>
     <row r="26" spans="1:20" ht="9" customHeight="1">
-      <c r="A26" s="39"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="40"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="39"/>
     </row>
     <row r="27" spans="1:20" ht="28.5" customHeight="1">
-      <c r="A27" s="41"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="35"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="46"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="34"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="45"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="48"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="49"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2169,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:BN53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2184,7 +2361,7 @@
     <col min="5" max="5" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="39" customHeight="1">
+    <row r="1" spans="1:66" s="7" customFormat="1" ht="39" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2200,8 +2377,69 @@
       <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="56"/>
+      <c r="AN1" s="56"/>
+      <c r="AO1" s="56"/>
+      <c r="AP1" s="56"/>
+      <c r="AQ1" s="56"/>
+      <c r="AR1" s="56"/>
+      <c r="AS1" s="56"/>
+      <c r="AT1" s="56"/>
+      <c r="AU1" s="56"/>
+      <c r="AV1" s="56"/>
+      <c r="AW1" s="56"/>
+      <c r="AX1" s="56"/>
+      <c r="AY1" s="56"/>
+      <c r="AZ1" s="56"/>
+      <c r="BA1" s="56"/>
+      <c r="BB1" s="56"/>
+      <c r="BC1" s="56"/>
+      <c r="BD1" s="56"/>
+      <c r="BE1" s="56"/>
+      <c r="BF1" s="56"/>
+      <c r="BG1" s="56"/>
+      <c r="BH1" s="56"/>
+      <c r="BI1" s="56"/>
+      <c r="BJ1" s="56"/>
+      <c r="BK1" s="56"/>
+      <c r="BL1" s="56"/>
+      <c r="BM1" s="56"/>
+      <c r="BN1" s="56"/>
+    </row>
+    <row r="2" spans="1:66">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -2210,7 +2448,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:66">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -2219,7 +2457,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:66">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -2228,7 +2466,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:66">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
@@ -2237,14 +2475,14 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:66">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:66">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2253,7 +2491,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:66">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -2262,7 +2500,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:66">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -2271,7 +2509,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:66">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -2280,7 +2518,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:66">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -2289,7 +2527,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:66">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
@@ -2298,7 +2536,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:66">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
@@ -2307,7 +2545,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:66">
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
@@ -2316,7 +2554,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:66">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
@@ -2325,7 +2563,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:66">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -2662,4 +2900,369 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="5" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="J2" s="57"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75">
+      <c r="B3" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="57"/>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="J4" s="57"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="58"/>
+      <c r="J5" s="57"/>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="68"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="70">
+        <f>G21</f>
+        <v>5000</v>
+      </c>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72">
+        <v>12</v>
+      </c>
+      <c r="H6" s="70">
+        <f>E6*G6</f>
+        <v>60000</v>
+      </c>
+      <c r="I6" s="71"/>
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="68"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="70">
+        <v>2500</v>
+      </c>
+      <c r="F7" s="71"/>
+      <c r="G7" s="72">
+        <v>12</v>
+      </c>
+      <c r="H7" s="70">
+        <f>E7*G7</f>
+        <v>30000</v>
+      </c>
+      <c r="I7" s="71"/>
+      <c r="J7" s="57"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="68"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="70">
+        <v>1000</v>
+      </c>
+      <c r="F8" s="71"/>
+      <c r="G8" s="72">
+        <v>12</v>
+      </c>
+      <c r="H8" s="70">
+        <f>E8*G8</f>
+        <v>12000</v>
+      </c>
+      <c r="I8" s="71"/>
+      <c r="J8" s="57"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="68"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="70">
+        <v>-2000</v>
+      </c>
+      <c r="I9" s="71"/>
+      <c r="J9" s="57"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="62">
+        <f>SUM(H6:I9)</f>
+        <v>100000</v>
+      </c>
+      <c r="I10" s="63"/>
+      <c r="J10" s="57"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+    </row>
+    <row r="14" spans="2:10" ht="15.75">
+      <c r="B14" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="58"/>
+      <c r="G16" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="63"/>
+      <c r="J16" s="57"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="60"/>
+      <c r="D17" s="61">
+        <v>1</v>
+      </c>
+      <c r="E17" s="69">
+        <v>1000</v>
+      </c>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70">
+        <f>D17*E17</f>
+        <v>1000</v>
+      </c>
+      <c r="H17" s="71"/>
+      <c r="J17" s="57"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="60"/>
+      <c r="D18" s="61">
+        <v>1</v>
+      </c>
+      <c r="E18" s="69">
+        <v>900</v>
+      </c>
+      <c r="F18" s="69"/>
+      <c r="G18" s="70">
+        <f>D18*E18</f>
+        <v>900</v>
+      </c>
+      <c r="H18" s="71"/>
+      <c r="J18" s="57"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="60"/>
+      <c r="D19" s="61">
+        <v>2</v>
+      </c>
+      <c r="E19" s="69">
+        <v>850</v>
+      </c>
+      <c r="F19" s="69"/>
+      <c r="G19" s="70">
+        <f>D19*E19</f>
+        <v>1700</v>
+      </c>
+      <c r="H19" s="71"/>
+      <c r="J19" s="57"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="60"/>
+      <c r="D20" s="61">
+        <v>2</v>
+      </c>
+      <c r="E20" s="69">
+        <v>700</v>
+      </c>
+      <c r="F20" s="69"/>
+      <c r="G20" s="70">
+        <f>D20*E20</f>
+        <v>1400</v>
+      </c>
+      <c r="H20" s="71"/>
+      <c r="J20" s="57"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="62">
+        <f>SUM(G17:H20)</f>
+        <v>5000</v>
+      </c>
+      <c r="H21" s="63"/>
+      <c r="J21" s="57"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>